<commit_message>
Final weight script and update
- Sostituito "Verona" con "Hellas Verona" in "Calendario_2021.xlsx".
- Implementato l'algoritmo che calcola il "peso" da aggiungere alla predizione del singolo giocatore.
</commit_message>
<xml_diff>
--- a/Dataset/Calendario_2021.xlsx
+++ b/Dataset/Calendario_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UniDispense\ICON\ICON_Project\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F13AF44-8CF6-4AD0-998B-60E9B6A86AD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02495F65-DE34-413A-89C5-C6B7763A74C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Udinese-Spezia</t>
   </si>
   <si>
-    <t>Verona-Roma</t>
-  </si>
-  <si>
     <t>Bologna-Parma</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Torino-Atalanta</t>
   </si>
   <si>
-    <t>Verona-Udinese</t>
-  </si>
-  <si>
     <t>Atalanta-Cagliari</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>Crotone-Lazio</t>
   </si>
   <si>
-    <t>Atalanta-Verona</t>
-  </si>
-  <si>
     <t>Crotone-Napoli</t>
   </si>
   <si>
@@ -183,9 +174,6 @@
     <t>Fiorentina-Cagliari</t>
   </si>
   <si>
-    <t>Bologna-Verona</t>
-  </si>
-  <si>
     <t>Fiorentina-Crotone</t>
   </si>
   <si>
@@ -270,9 +258,6 @@
     <t>Inter-Napoli</t>
   </si>
   <si>
-    <t>Fiorentina-Verona</t>
-  </si>
-  <si>
     <t>Milan-Lazio</t>
   </si>
   <si>
@@ -348,9 +333,6 @@
     <t>Sampdoria-Lazio</t>
   </si>
   <si>
-    <t>Juventus-Verona</t>
-  </si>
-  <si>
     <t>Sampdoria-Genoa</t>
   </si>
   <si>
@@ -366,9 +348,6 @@
     <t>Roma-Sassuolo</t>
   </si>
   <si>
-    <t>Lazio-Verona</t>
-  </si>
-  <si>
     <t>Parma-Cagliari</t>
   </si>
   <si>
@@ -405,9 +384,6 @@
     <t>Spezia-Juventus</t>
   </si>
   <si>
-    <t>Milan-Verona</t>
-  </si>
-  <si>
     <t>Sampdoria-Bologna</t>
   </si>
   <si>
@@ -444,9 +420,6 @@
     <t>Parma-Sampdoria</t>
   </si>
   <si>
-    <t>Parma-Verona</t>
-  </si>
-  <si>
     <t>Torino-Cagliari</t>
   </si>
   <si>
@@ -555,46 +528,73 @@
     <t>Sassuolo-Torino</t>
   </si>
   <si>
-    <t>Verona-Benevento</t>
-  </si>
-  <si>
     <t>Torino-Crotone</t>
   </si>
   <si>
-    <t>Verona-Sassuolo</t>
-  </si>
-  <si>
     <t>Torino-Sampdoria</t>
   </si>
   <si>
-    <t>Verona-Cagliari</t>
-  </si>
-  <si>
     <t>Torino-Udinese</t>
   </si>
   <si>
-    <t>Verona-Sampdoria</t>
-  </si>
-  <si>
     <t>Torino-Bologna</t>
   </si>
   <si>
-    <t>Verona-Inter</t>
-  </si>
-  <si>
-    <t>Spezia-Verona</t>
-  </si>
-  <si>
-    <t>Torino-Verona</t>
-  </si>
-  <si>
-    <t>Verona-Crotone</t>
-  </si>
-  <si>
     <t>Torino-Spezia</t>
   </si>
   <si>
-    <t>Verona-Napoli</t>
+    <t>Atalanta-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Bologna-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Fiorentina-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Juventus-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Lazio-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Milan-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Parma-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Roma</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Udinese</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Benevento</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Sassuolo</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Cagliari</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Sampdoria</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Inter</t>
+  </si>
+  <si>
+    <t>Spezia-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Torino-Hellas Verona</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Crotone</t>
+  </si>
+  <si>
+    <t>Hellas Verona-Napoli</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1330,115 +1330,115 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="V2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:38" ht="15" customHeight="1">
@@ -1446,115 +1446,115 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="R3" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AK3" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AL3" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:38" ht="15" customHeight="1">
@@ -1562,115 +1562,115 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AJ4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AK4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AL4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:38" ht="15" customHeight="1">
@@ -1678,115 +1678,115 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="M5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AH5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AI5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AJ5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AK5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AL5" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL5" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:38" ht="15" customHeight="1">
@@ -1794,115 +1794,115 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AE6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AG6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AH6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AI6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AK6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AL6" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="AH6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AI6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AK6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AL6" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1">
@@ -1910,115 +1910,115 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="K7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE7" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="AF7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AG7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AH7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AI7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AJ7" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AK7" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AL7" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="AF7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG7" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH7" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AJ7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="AK7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL7" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1">
@@ -2026,115 +2026,115 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD8" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="AE8" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="AF8" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="AG8" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="AH8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AI8" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AJ8" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AK8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AL8" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="AE8" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF8" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AG8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AH8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AI8" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AJ8" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AK8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AL8" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1">
@@ -2142,115 +2142,115 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE9" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="AF9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="AG9" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="Y9" s="1" t="s">
+      <c r="AH9" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="Z9" s="1" t="s">
+      <c r="AI9" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AJ9" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AK9" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AC9" s="1" t="s">
+      <c r="AL9" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AF9" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG9" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AH9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AI9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AJ9" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="AK9" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AL9" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1">
@@ -2258,228 +2258,228 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE10" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="AF10" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="AG10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="Y10" s="1" t="s">
+      <c r="AH10" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="Z10" s="1" t="s">
+      <c r="AI10" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AJ10" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AK10" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AC10" s="1" t="s">
+      <c r="AL10" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="AD10" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="AE10" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AF10" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG10" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="AH10" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="AI10" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="AJ10" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AK10" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="AL10" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:38" ht="15" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>179</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>189</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>9</v>
+        <v>179</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>19</v>
+        <v>180</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="AL11" s="1" t="s">
         <v>189</v>

</xml_diff>